<commit_message>
Llamados completos li completo
</commit_message>
<xml_diff>
--- a/Id ufc.xlsx
+++ b/Id ufc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Google Drive\Universidad\Semestre 7 y 8\Semestre 7\Ingenieria web\Portafolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AC5451-7073-48E6-A96A-CAB3EE86FA5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39927727-FCBC-481F-860E-34AABA7DA2F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E68CBB25-667E-4763-9B50-9DD8531A95CF}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{E68CBB25-667E-4763-9B50-9DD8531A95CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="130">
   <si>
     <t>Aljamain sterling</t>
   </si>
@@ -42,9 +42,6 @@
     <t>alexander volkanovski</t>
   </si>
   <si>
-    <t>Ligero : sin campeon</t>
-  </si>
-  <si>
     <t>Kamaru usman</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>Rogeiro Bontorin</t>
   </si>
   <si>
-    <t>Tim Elliot</t>
-  </si>
-  <si>
     <t>Top 10 Gallo M</t>
   </si>
   <si>
@@ -222,9 +216,6 @@
     <t>Jorge Masvidal</t>
   </si>
   <si>
-    <t>Stephen Thompson</t>
-  </si>
-  <si>
     <t>Vicente Luque</t>
   </si>
   <si>
@@ -237,9 +228,6 @@
     <t>Neil Magny</t>
   </si>
   <si>
-    <t>Tyron Woodley</t>
-  </si>
-  <si>
     <t>Robert Whittaker</t>
   </si>
   <si>
@@ -354,9 +342,6 @@
     <t>Carla Esparza</t>
   </si>
   <si>
-    <t>Nina Nunes</t>
-  </si>
-  <si>
     <t>Marina Rodriguez</t>
   </si>
   <si>
@@ -369,9 +354,6 @@
     <t>Tecia Torres</t>
   </si>
   <si>
-    <t>Amanda Ribas</t>
-  </si>
-  <si>
     <t>Jessica Andrade</t>
   </si>
   <si>
@@ -435,13 +417,13 @@
     <t>Alexandre Pantoja</t>
   </si>
   <si>
-    <t>Joseph Benavidez</t>
-  </si>
-  <si>
     <t>Kai Kara-France</t>
   </si>
   <si>
     <t>Petr Yan</t>
+  </si>
+  <si>
+    <t>Alexa Grasso</t>
   </si>
 </sst>
 </file>
@@ -450,7 +432,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -508,13 +490,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -831,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F34A85-BBE1-48FE-96C1-6101CDC6CE5E}">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -847,46 +829,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="D1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="3"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="6"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="K1" s="3"/>
+      <c r="J1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1">
         <v>140000613</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H2" s="1">
         <v>140000521</v>
       </c>
       <c r="J2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="K2" s="1">
         <v>140000350</v>
@@ -894,25 +876,25 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>140000215</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1">
         <v>140000614</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H3" s="1">
         <v>140000526</v>
       </c>
       <c r="J3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K3" s="1">
         <v>140000634</v>
@@ -926,19 +908,19 @@
         <v>140000086</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E4" s="1">
         <v>140000258</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H4" s="1">
         <v>140000195</v>
       </c>
       <c r="J4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K4" s="1">
         <v>140000394</v>
@@ -952,19 +934,19 @@
         <v>140000347</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1">
         <v>140000222</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H5" s="1">
         <v>140000196</v>
       </c>
       <c r="J5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="K5" s="1">
         <v>140000296</v>
@@ -974,23 +956,26 @@
       <c r="A6" t="s">
         <v>2</v>
       </c>
+      <c r="B6" s="1">
+        <v>140000145</v>
+      </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1">
-        <v>140000019</v>
+        <v>140000910</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="1">
-        <v>140000221</v>
+        <v>140000089</v>
       </c>
       <c r="J6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="K6" s="1">
-        <v>140000398</v>
+        <v>140000235</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -998,25 +983,25 @@
         <v>3</v>
       </c>
       <c r="B7" s="1">
-        <v>140000145</v>
+        <v>140000074</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>127</v>
       </c>
       <c r="E7" s="1">
-        <v>140000910</v>
+        <v>140000059</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H7" s="1">
-        <v>140000089</v>
+        <v>140000444</v>
       </c>
       <c r="J7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="K7" s="1">
-        <v>140000235</v>
+        <v>140000441</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1027,22 +1012,22 @@
         <v>140000074</v>
       </c>
       <c r="D8" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1">
-        <v>140000059</v>
+        <v>140000152</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H8" s="1">
-        <v>140000444</v>
+        <v>140000047</v>
       </c>
       <c r="J8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="K8" s="1">
-        <v>140000441</v>
+        <v>140000240</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1050,25 +1035,25 @@
         <v>5</v>
       </c>
       <c r="B9" s="1">
-        <v>140000074</v>
+        <v>140000098</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="1">
-        <v>140000152</v>
+        <v>140000028</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H9" s="1">
-        <v>140000047</v>
+        <v>140000752</v>
       </c>
       <c r="J9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K9" s="1">
-        <v>140000240</v>
+        <v>140000140</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1076,53 +1061,54 @@
         <v>6</v>
       </c>
       <c r="B10" s="1">
-        <v>140000098</v>
-      </c>
-      <c r="D10" t="s">
+        <v>140000141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1">
+        <v>140000402</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="1">
-        <v>140000028</v>
-      </c>
-      <c r="G10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="1">
-        <v>140000752</v>
-      </c>
-      <c r="J10" t="s">
-        <v>110</v>
-      </c>
-      <c r="K10" s="1">
-        <v>140000140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="1">
-        <v>140000632</v>
-      </c>
-      <c r="G11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="1">
-        <v>140000144</v>
-      </c>
-      <c r="J11" t="s">
-        <v>111</v>
-      </c>
-      <c r="K11" s="1">
-        <v>140000432</v>
-      </c>
+      <c r="E11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1">
-        <v>140000141</v>
+        <v>140000446</v>
+      </c>
+      <c r="D12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="1">
+        <v>140000116</v>
+      </c>
+      <c r="G12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="1">
+        <v>140000630</v>
+      </c>
+      <c r="J12" t="s">
+        <v>106</v>
+      </c>
+      <c r="K12" s="1">
+        <v>140000349</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1130,72 +1116,65 @@
         <v>8</v>
       </c>
       <c r="B13" s="1">
-        <v>140000402</v>
-      </c>
-      <c r="D13" s="3" t="s">
+        <v>140000446</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1">
+        <v>140000007</v>
+      </c>
+      <c r="G13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="1">
+        <v>140000556</v>
+      </c>
+      <c r="J13" t="s">
+        <v>107</v>
+      </c>
+      <c r="K13" s="1">
+        <v>140000389</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="D14" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="G13" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1">
-        <v>140000446</v>
-      </c>
-      <c r="D14" t="s">
-        <v>135</v>
-      </c>
       <c r="E14" s="1">
-        <v>140000116</v>
+        <v>140000668</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H14" s="1">
-        <v>140000630</v>
+        <v>140000348</v>
       </c>
       <c r="J14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="K14" s="1">
-        <v>140000349</v>
+        <v>140000517</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1">
-        <v>140000446</v>
-      </c>
       <c r="D15" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="1">
-        <v>140000007</v>
+        <v>140000139</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H15" s="1">
-        <v>140000556</v>
+        <v>140000329</v>
       </c>
       <c r="J15" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K15" s="1">
-        <v>140000389</v>
+        <v>140000205</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1203,19 +1182,19 @@
         <v>24</v>
       </c>
       <c r="E16" s="1">
-        <v>140000668</v>
+        <v>140000049</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H16" s="1">
-        <v>140000348</v>
+        <v>140000197</v>
       </c>
       <c r="J16" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K16" s="1">
-        <v>140000517</v>
+        <v>140000094</v>
       </c>
     </row>
     <row r="17" spans="4:11">
@@ -1223,19 +1202,19 @@
         <v>25</v>
       </c>
       <c r="E17" s="1">
-        <v>140000139</v>
+        <v>140000052</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H17" s="1">
-        <v>140000329</v>
+        <v>140000467</v>
       </c>
       <c r="J17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K17" s="1">
-        <v>140000205</v>
+        <v>140000011</v>
       </c>
     </row>
     <row r="18" spans="4:11">
@@ -1243,19 +1222,19 @@
         <v>26</v>
       </c>
       <c r="E18" s="1">
-        <v>140000049</v>
+        <v>140000504</v>
       </c>
       <c r="G18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H18" s="1">
-        <v>140000197</v>
+        <v>140000245</v>
       </c>
       <c r="J18" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="K18" s="1">
-        <v>140000094</v>
+        <v>140000333</v>
       </c>
     </row>
     <row r="19" spans="4:11">
@@ -1263,19 +1242,19 @@
         <v>27</v>
       </c>
       <c r="E19" s="1">
-        <v>140000052</v>
+        <v>140000138</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H19" s="1">
-        <v>140000467</v>
+        <v>140000265</v>
       </c>
       <c r="J19" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="K19" s="1">
-        <v>140000011</v>
+        <v>140000403</v>
       </c>
     </row>
     <row r="20" spans="4:11">
@@ -1283,19 +1262,19 @@
         <v>28</v>
       </c>
       <c r="E20" s="1">
-        <v>140000504</v>
+        <v>140000907</v>
       </c>
       <c r="G20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H20" s="1">
-        <v>140000245</v>
+        <v>140000604</v>
       </c>
       <c r="J20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K20" s="1">
-        <v>140000333</v>
+        <v>140000281</v>
       </c>
     </row>
     <row r="21" spans="4:11">
@@ -1303,88 +1282,94 @@
         <v>29</v>
       </c>
       <c r="E21" s="1">
-        <v>140000138</v>
+        <v>140000051</v>
       </c>
       <c r="G21" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="1">
+        <v>140000229</v>
+      </c>
+      <c r="J21" t="s">
+        <v>129</v>
+      </c>
+      <c r="K21" s="1">
+        <v>140000397</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11">
+      <c r="D23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="G23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="4:11">
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="1">
+        <v>140000267</v>
+      </c>
+      <c r="G24" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="1">
+        <v>140000015</v>
+      </c>
+      <c r="J24" t="s">
+        <v>115</v>
+      </c>
+      <c r="K24" s="1">
+        <v>140000471</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11">
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="1">
+        <v>140000712</v>
+      </c>
+      <c r="G25" t="s">
         <v>75</v>
       </c>
-      <c r="H21" s="1">
-        <v>140000265</v>
-      </c>
-      <c r="J21" t="s">
-        <v>119</v>
-      </c>
-      <c r="K21" s="1">
-        <v>140000403</v>
-      </c>
-    </row>
-    <row r="22" spans="4:11">
-      <c r="D22" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="1">
-        <v>140000907</v>
-      </c>
-      <c r="G22" t="s">
-        <v>76</v>
-      </c>
-      <c r="H22" s="1">
-        <v>140000604</v>
-      </c>
-      <c r="J22" t="s">
-        <v>120</v>
-      </c>
-      <c r="K22" s="1">
-        <v>140000281</v>
-      </c>
-    </row>
-    <row r="23" spans="4:11">
-      <c r="D23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="1">
-        <v>140000051</v>
-      </c>
-      <c r="G23" t="s">
-        <v>77</v>
-      </c>
-      <c r="H23" s="1">
-        <v>140000229</v>
-      </c>
-    </row>
-    <row r="25" spans="4:11">
-      <c r="D25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="G25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="K25" s="3"/>
+      <c r="H25" s="1">
+        <v>140000387</v>
+      </c>
+      <c r="J25" t="s">
+        <v>116</v>
+      </c>
+      <c r="K25" s="1">
+        <v>140000447</v>
+      </c>
     </row>
     <row r="26" spans="4:11">
       <c r="D26" t="s">
         <v>33</v>
       </c>
       <c r="E26" s="1">
-        <v>140000267</v>
+        <v>140000137</v>
       </c>
       <c r="G26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H26" s="1">
-        <v>140000015</v>
+        <v>140000193</v>
       </c>
       <c r="J26" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K26" s="1">
-        <v>140000471</v>
+        <v>140000359</v>
       </c>
     </row>
     <row r="27" spans="4:11">
@@ -1392,19 +1377,19 @@
         <v>34</v>
       </c>
       <c r="E27" s="1">
-        <v>140000712</v>
+        <v>140000615</v>
       </c>
       <c r="G27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H27" s="1">
-        <v>140000387</v>
+        <v>140000124</v>
       </c>
       <c r="J27" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K27" s="1">
-        <v>140000447</v>
+        <v>140000345</v>
       </c>
     </row>
     <row r="28" spans="4:11">
@@ -1412,19 +1397,19 @@
         <v>35</v>
       </c>
       <c r="E28" s="1">
-        <v>140000137</v>
+        <v>140000421</v>
       </c>
       <c r="G28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H28" s="1">
-        <v>140000193</v>
+        <v>140000918</v>
       </c>
       <c r="J28" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K28" s="1">
-        <v>140000359</v>
+        <v>140000159</v>
       </c>
     </row>
     <row r="29" spans="4:11">
@@ -1432,19 +1417,19 @@
         <v>36</v>
       </c>
       <c r="E29" s="1">
-        <v>140000615</v>
+        <v>140000396</v>
       </c>
       <c r="G29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H29" s="1">
-        <v>140000124</v>
+        <v>140000147</v>
       </c>
       <c r="J29" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K29" s="1">
-        <v>140000345</v>
+        <v>140000462</v>
       </c>
     </row>
     <row r="30" spans="4:11">
@@ -1452,19 +1437,19 @@
         <v>37</v>
       </c>
       <c r="E30" s="1">
-        <v>140000421</v>
+        <v>140000243</v>
       </c>
       <c r="G30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H30" s="1">
-        <v>140000918</v>
+        <v>140000113</v>
       </c>
       <c r="J30" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="K30" s="1">
-        <v>140000159</v>
+        <v>140000710</v>
       </c>
     </row>
     <row r="31" spans="4:11">
@@ -1472,19 +1457,19 @@
         <v>38</v>
       </c>
       <c r="E31" s="1">
-        <v>140000396</v>
+        <v>140000178</v>
       </c>
       <c r="G31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H31" s="1">
-        <v>140000147</v>
+        <v>140000192</v>
       </c>
       <c r="J31" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K31" s="1">
-        <v>140000462</v>
+        <v>140000701</v>
       </c>
     </row>
     <row r="32" spans="4:11">
@@ -1492,19 +1477,19 @@
         <v>39</v>
       </c>
       <c r="E32" s="1">
-        <v>140000243</v>
+        <v>140000136</v>
       </c>
       <c r="G32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H32" s="1">
-        <v>140000113</v>
+        <v>140000261</v>
       </c>
       <c r="J32" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K32" s="1">
-        <v>140000710</v>
+        <v>140000128</v>
       </c>
     </row>
     <row r="33" spans="4:11">
@@ -1512,91 +1497,79 @@
         <v>40</v>
       </c>
       <c r="E33" s="1">
-        <v>140000178</v>
+        <v>140000024</v>
       </c>
       <c r="G33" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="1">
+        <v>140000043</v>
+      </c>
+      <c r="J33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K33" s="5">
+        <v>140000380</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11">
+      <c r="D35" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" s="6"/>
+      <c r="G35" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="K35" s="6"/>
+    </row>
+    <row r="36" spans="4:11">
+      <c r="D36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="1">
+        <v>140000266</v>
+      </c>
+      <c r="G36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H36" s="1">
+        <v>140000558</v>
+      </c>
+      <c r="J36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11">
+      <c r="D37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="1">
+        <v>140000247</v>
+      </c>
+      <c r="G37" t="s">
         <v>85</v>
       </c>
-      <c r="H33" s="1">
-        <v>140000192</v>
-      </c>
-      <c r="J33" t="s">
-        <v>128</v>
-      </c>
-      <c r="K33" s="1">
-        <v>140000701</v>
-      </c>
-    </row>
-    <row r="34" spans="4:11">
-      <c r="D34" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="1">
-        <v>140000136</v>
-      </c>
-      <c r="G34" t="s">
-        <v>86</v>
-      </c>
-      <c r="H34" s="1">
-        <v>140000261</v>
-      </c>
-      <c r="J34" t="s">
-        <v>129</v>
-      </c>
-      <c r="K34" s="1">
-        <v>140000128</v>
-      </c>
-    </row>
-    <row r="35" spans="4:11">
-      <c r="D35" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" s="1">
-        <v>140000024</v>
-      </c>
-      <c r="G35" t="s">
-        <v>87</v>
-      </c>
-      <c r="H35" s="1">
-        <v>140000043</v>
-      </c>
-      <c r="J35" t="s">
-        <v>130</v>
-      </c>
-      <c r="K35" s="6">
-        <v>140000380</v>
-      </c>
-    </row>
-    <row r="37" spans="4:11">
-      <c r="D37" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37" s="3"/>
-      <c r="G37" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H37" s="3"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="K37" s="3"/>
+      <c r="H37" s="1">
+        <v>140000173</v>
+      </c>
     </row>
     <row r="38" spans="4:11">
       <c r="D38" t="s">
         <v>44</v>
       </c>
       <c r="E38" s="1">
-        <v>140000266</v>
+        <v>140000045</v>
       </c>
       <c r="G38" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H38" s="1">
-        <v>140000558</v>
-      </c>
-      <c r="J38" t="s">
-        <v>131</v>
+        <v>140000218</v>
       </c>
     </row>
     <row r="39" spans="4:11">
@@ -1604,13 +1577,13 @@
         <v>45</v>
       </c>
       <c r="E39" s="1">
-        <v>140000247</v>
+        <v>140001095</v>
       </c>
       <c r="G39" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H39" s="1">
-        <v>140000173</v>
+        <v>140000534</v>
       </c>
     </row>
     <row r="40" spans="4:11">
@@ -1618,13 +1591,13 @@
         <v>46</v>
       </c>
       <c r="E40" s="1">
-        <v>140000045</v>
+        <v>140000401</v>
       </c>
       <c r="G40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H40" s="1">
-        <v>140000218</v>
+        <v>140000647</v>
       </c>
     </row>
     <row r="41" spans="4:11">
@@ -1632,13 +1605,13 @@
         <v>47</v>
       </c>
       <c r="E41" s="1">
-        <v>140001095</v>
+        <v>140000867</v>
       </c>
       <c r="G41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H41" s="1">
-        <v>140000534</v>
+        <v>140000034</v>
       </c>
     </row>
     <row r="42" spans="4:11">
@@ -1646,13 +1619,13 @@
         <v>48</v>
       </c>
       <c r="E42" s="1">
-        <v>140000401</v>
+        <v>140000368</v>
       </c>
       <c r="G42" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H42" s="1">
-        <v>140000647</v>
+        <v>140000271</v>
       </c>
     </row>
     <row r="43" spans="4:11">
@@ -1660,13 +1633,13 @@
         <v>49</v>
       </c>
       <c r="E43" s="1">
-        <v>140000867</v>
+        <v>140000487</v>
       </c>
       <c r="G43" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H43" s="1">
-        <v>140000034</v>
+        <v>140000323</v>
       </c>
     </row>
     <row r="44" spans="4:11">
@@ -1674,13 +1647,13 @@
         <v>50</v>
       </c>
       <c r="E44" s="1">
-        <v>140000368</v>
+        <v>140000165</v>
       </c>
       <c r="G44" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H44" s="1">
-        <v>140000271</v>
+        <v>140000299</v>
       </c>
     </row>
     <row r="45" spans="4:11">
@@ -1688,68 +1661,40 @@
         <v>51</v>
       </c>
       <c r="E45" s="1">
-        <v>140000487</v>
+        <v>140000096</v>
       </c>
       <c r="G45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H45" s="1">
-        <v>140000323</v>
-      </c>
-    </row>
-    <row r="46" spans="4:11">
-      <c r="D46" t="s">
-        <v>52</v>
-      </c>
-      <c r="E46" s="1">
-        <v>140000165</v>
-      </c>
-      <c r="G46" t="s">
-        <v>96</v>
-      </c>
-      <c r="H46" s="1">
-        <v>140000299</v>
+        <v>140000992</v>
       </c>
     </row>
     <row r="47" spans="4:11">
-      <c r="D47" t="s">
-        <v>53</v>
-      </c>
-      <c r="E47" s="1">
-        <v>140000096</v>
-      </c>
-      <c r="G47" t="s">
-        <v>97</v>
-      </c>
-      <c r="H47" s="1">
-        <v>140000992</v>
-      </c>
-    </row>
-    <row r="49" spans="5:11">
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-    </row>
-    <row r="50" spans="5:11">
-      <c r="E50" s="5">
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+    </row>
+    <row r="48" spans="4:11">
+      <c r="E48" s="4">
         <v>1400000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="J47:K47"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J35:K35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>